<commit_message>
Bom STD Qty modified for M3x8 and X10
</commit_message>
<xml_diff>
--- a/bom/BOM_XY_STD.xlsx
+++ b/bom/BOM_XY_STD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{7AB44BD0-E2BA-4338-8728-1559E83C9B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{72B39E02-27B5-487B-9D1A-93339FD3B02D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C37BC-20B5-4F56-BA6D-1DDF7E987E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3576,29 +3576,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="84.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="85" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="34" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="43.5703125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="2"/>
+    <col min="4" max="4" width="16.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7265625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.26953125" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="43.54296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>81</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>90</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>85</v>
       </c>
@@ -3677,7 +3677,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>85</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>85</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>85</v>
       </c>
@@ -3764,7 +3764,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>85</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>85</v>
       </c>
@@ -3820,7 +3820,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>85</v>
       </c>
@@ -3849,7 +3849,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>85</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>85</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>85</v>
       </c>
@@ -3934,7 +3934,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>85</v>
       </c>
@@ -3963,7 +3963,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>85</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="J14" s="9"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>85</v>
       </c>
@@ -4019,7 +4019,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>85</v>
       </c>
@@ -4040,13 +4040,13 @@
         <v>6</v>
       </c>
       <c r="H16" s="37">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="9"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>85</v>
       </c>
@@ -4067,13 +4067,13 @@
         <v>6</v>
       </c>
       <c r="H17" s="37">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I17" s="41"/>
       <c r="J17" s="9"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>85</v>
       </c>
@@ -4100,7 +4100,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>85</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="46" t="s">
         <v>85</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="J20" s="14"/>
       <c r="K20" s="47"/>
     </row>
-    <row r="21" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="57" t="s">
         <v>85</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="J21" s="60"/>
       <c r="K21" s="60"/>
     </row>
-    <row r="22" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>85</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="57" t="s">
         <v>85</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="48" t="s">
         <v>85</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="J24" s="51"/>
       <c r="K24" s="56"/>
     </row>
-    <row r="25" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>85</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>85</v>
       </c>
@@ -4328,7 +4328,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>85</v>
       </c>
@@ -4355,7 +4355,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>85</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>85</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>85</v>
       </c>
@@ -4436,7 +4436,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>85</v>
       </c>
@@ -4463,7 +4463,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>85</v>
       </c>
@@ -4490,7 +4490,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>85</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>85</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>85</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
         <v>85</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
         <v>85</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
         <v>85</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
         <v>85</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
         <v>85</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
         <v>85</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
         <v>85</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
         <v>85</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>85</v>
       </c>

</xml_diff>